<commit_message>
Cambios en el mapeo
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\codigoqr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F078348F-926C-4C30-9114-6AFD3E6F6FEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DB3F90-56F6-46BC-A04E-F137AAF266B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -67,9 +67,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>1010111</t>
-  </si>
-  <si>
     <t>4321</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>406-740100-05</t>
   </si>
   <si>
-    <t>userqa10</t>
-  </si>
-  <si>
     <t>monto</t>
   </si>
   <si>
@@ -149,18 +143,37 @@
   </si>
   <si>
     <t>406-785280-05</t>
+  </si>
+  <si>
+    <t>userrobot2</t>
+  </si>
+  <si>
+    <t>22483228</t>
+  </si>
+  <si>
+    <t>406-132280-02</t>
+  </si>
+  <si>
+    <t>150000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -234,21 +247,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -556,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -617,252 +632,252 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="11" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>15</v>
+      <c r="B2" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="11" customFormat="1">
       <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>15</v>
+      <c r="B3" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="O3" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="11">
-        <v>120000</v>
+        <v>39</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>15</v>
+        <v>35</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="H4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="O4" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>15</v>
+        <v>38</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="7" t="s">
+      <c r="P5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:19">

</xml_diff>

<commit_message>
Estabilizacion pago de tarjetas de credito
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS\src\test\resources\datadriven\codigoqr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\codigoqr\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17B28FF-29BE-4BF4-A356-AB3A2F3D75C2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -138,22 +139,35 @@
     <t>43024987</t>
   </si>
   <si>
-    <t>automata87</t>
-  </si>
-  <si>
-    <t>406-749870-13</t>
+    <t>autotest10</t>
+  </si>
+  <si>
+    <t>Corriente</t>
+  </si>
+  <si>
+    <t>406-125170-00</t>
+  </si>
+  <si>
+    <t>406-725170-06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -241,23 +255,24 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -563,11 +578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -692,10 +707,10 @@
         <v>30</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="14" t="s">
         <v>40</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="S2" s="11" t="s">
         <v>32</v>
@@ -750,8 +765,8 @@
       <c r="P3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="14" t="s">
-        <v>40</v>
+      <c r="Q3" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="R3" s="12" t="s">
         <v>37</v>
@@ -807,10 +822,10 @@
         <v>31</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" s="14" t="s">
         <v>40</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="R4" s="11" t="s">
         <v>35</v>
@@ -868,8 +883,8 @@
       <c r="P5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="Q5" s="14" t="s">
-        <v>40</v>
+      <c r="Q5" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="R5" s="11"/>
       <c r="S5" s="11" t="s">
@@ -884,10 +899,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="N3" r:id="rId2"/>
-    <hyperlink ref="N4" r:id="rId3"/>
-    <hyperlink ref="N5" r:id="rId4"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>

</xml_diff>

<commit_message>
Cambios mapeos codigo qr
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS\src\test\resources\datadriven\codigoqr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\codigoqr\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C74CC05-84D6-4914-8538-04592E45ECE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -90,9 +91,6 @@
     <t>jalzate@todo1.net</t>
   </si>
   <si>
-    <t>1234</t>
-  </si>
-  <si>
     <t>Acierto</t>
   </si>
   <si>
@@ -135,25 +133,41 @@
     <t>150000</t>
   </si>
   <si>
-    <t>43024987</t>
-  </si>
-  <si>
-    <t>automata87</t>
-  </si>
-  <si>
-    <t>406-749870-13</t>
+    <t>406-139440-02</t>
+  </si>
+  <si>
+    <t>406-739440-04</t>
+  </si>
+  <si>
+    <t>406-739440-03</t>
+  </si>
+  <si>
+    <t>userrobot9</t>
+  </si>
+  <si>
+    <t>6789</t>
+  </si>
+  <si>
+    <t>22493944</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -241,24 +255,25 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -563,11 +578,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -630,42 +645,42 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="11" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>38</v>
+      <c r="B2" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>16</v>
@@ -689,39 +704,39 @@
         <v>22</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="11" customFormat="1">
       <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>38</v>
+      <c r="B3" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>16</v>
@@ -745,42 +760,42 @@
         <v>22</v>
       </c>
       <c r="O3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>16</v>
@@ -804,42 +819,42 @@
         <v>22</v>
       </c>
       <c r="O4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>16</v>
@@ -863,31 +878,31 @@
         <v>22</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R5" s="11"/>
       <c r="S5" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="Q8" s="14"/>
+      <c r="Q8" s="13"/>
     </row>
     <row r="13" spans="1:19">
       <c r="M13" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="N3" r:id="rId2"/>
-    <hyperlink ref="N4" r:id="rId3"/>
-    <hyperlink ref="N5" r:id="rId4"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>

</xml_diff>

<commit_message>
cambios en encarpetado de features
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20130" windowHeight="7425"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>406-139740-02</t>
+  </si>
+  <si>
+    <t>userunico01</t>
+  </si>
+  <si>
+    <t>406-767340-26</t>
   </si>
   <si>
     <t>Orientacion</t>
@@ -187,22 +193,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,6 +209,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -240,23 +239,46 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,21 +300,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -301,12 +308,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -314,17 +329,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -345,31 +351,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,145 +525,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,6 +555,41 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -567,40 +608,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,6 +628,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -634,163 +651,152 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1120,13 +1126,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="5"/>
   <cols>
     <col min="13" max="13" width="12.125"/>
     <col min="14" max="14" width="18.375" customWidth="1"/>
@@ -1392,6 +1398,57 @@
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6456734</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1234</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4321</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>369</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1420,16 +1477,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1437,50 +1494,50 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solucion transacciones rutas criticas
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/codigoqr/GenerarCodigoQr.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TODO1\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\codigoqr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="3" r:id="rId1"/>
     <sheet name="Listas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -158,14 +163,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,158 +181,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,194 +201,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -556,252 +225,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -810,62 +237,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1123,26 +506,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="14" max="14" width="18.3333333333333" customWidth="1"/>
-    <col min="15" max="15" width="17.6666666666667" customWidth="1"/>
+    <col min="14" max="14" width="18.375" customWidth="1"/>
+    <col min="15" max="15" width="17.625" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:17">
+    <row r="1" spans="1:17" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1456,25 +839,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="14.8333333333333" customWidth="1"/>
-    <col min="3" max="3" width="12.1666666666667" customWidth="1"/>
-    <col min="4" max="4" width="17.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1519,7 +900,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -1527,23 +908,22 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>